<commit_message>
Add leaderboard version control with weekly position tracking
- Implement weekly snapshot system that captures leaderboard state every Sunday
- Add position change indicators (green up arrows, red down arrows, "NEW" badges)
- Display points gained since last week for each debater
- Consolidate all utilities in src/utils/ directory with @/ import alias
- Add visual legend explaining position change indicators
- Create test snapshot system for immediate demonstration
- Update package.json to support ES modules

Features:
- Weekly automatic snapshots stored in data/leaderboard-snapshots/
- IMDb-style position change visualization with arrows and numbers
- Historical comparison shows previous rank and points gained
- Clean utility file organization following Next.js conventions

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/debate_achievements.xlsx
+++ b/data/debate_achievements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tikaram/Downloads/Claude Code/students/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9E8BC3-065D-7448-B510-0F48942B37B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F0187B-2D2C-C842-95F6-7BE705E9071C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -180,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="K33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E40" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="E41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="275">
   <si>
     <t>Tournament Name</t>
   </si>
@@ -5645,12 +5645,84 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Asian Schools Debating Championship 2025</t>
+  </si>
+  <si>
+    <t>June 16-18, 2025</t>
+  </si>
+  <si>
+    <t>https://asdc2025.calicotab.com/asdc2025/</t>
+  </si>
+  <si>
+    <t>We are thrilled to announce the outstanding results of our debaters at the Asian Schools Debating Championship ASDC (2025), held from June 16-18!
+A huge congratulations to our Novice Champions: Adrian W. (HKIS), Audrey L. (HKIS), and Ryan Q. (HKIS)! This is a fantastic achievement and a testament to their hard work and skill.
+Further congratulations to the students who reached the Quarterfinals: Aiden T. (CIS), Jonathan H. (DBS), Pacey Q. (Dulwich), Samuel K. (CIS), Vir K. (HKIS), CECILIA L. (BISOG), and Theodore W. (HKIS). Reaching the elimination rounds in such a competitive tournament is a significant accomplishment.
+Our debaters also earned numerous individual speaker awards across various categories.
+In the Junior category, congratulations to Theodore W. (HKIS) for placing 3rd, CECILIA L. (BISOG) for 4th, Aiden T. (CIS) for 7th, and Samuel K. (CIS) for 8th Best Speaker.
+In the Novice category, well done to Jonathan H. (DBS) for 2nd, Theodore W. (HKIS) for 5th, CECILIA L. (BISOG) for 6th, Pacey Q. (Dulwich) for 8th, Aiden T. (CIS) for 11th, Samuel K. (CIS) for 13th, and Vir K. (HKIS) for 15th Best Speaker.
+In the Overall rankings, congratulations to Jonathan H. (DBS) for placing 5th, Theodore W. (HKIS) for 12th, CECILIA L. (BISOG) for 13th, Pacey Q. (Dulwich) for 15th, and Aiden T. (CIS) for 18th Best Speaker.
+We are incredibly proud of all our debaters for their dedication, perseverance, and exceptional performance at ASDC 2025. These results reflect their commitment to excellence. Well done everyone!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Novice Champions:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="EB Garamond"/>
+      </rPr>
+      <t>Adrian W. (HKIS)
+Audrey L. (HKIS)
+Ryan Q. (HKIS)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="EB Garamond"/>
+      </rPr>
+      <t xml:space="preserve">
+Quarterfinalists:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="EB Garamond"/>
+      </rPr>
+      <t>Aiden T. (CIS)
+Jonathan H. (DBS)
+Pacey Q. (Dulwich)
+Samuel K. (CIS)
+Vir K. (HKIS)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Junior 7th Best: Aiden T. (CIS)
+Junior 8th Best: Samuel K. (CIS)
+Novice 2nd Best: Jonathan H. (DBS)
+Novice 5th Best: Theodore W. (HKIS)
+Novice 8th Best: Pacey Q. (Dulwich)
+Novice 11th Best: Aiden T. (CIS)
+Novice 13th Best: Samuel K. (CIS)
+Novice 15th Best: Vir K. (HKIS)
+Overall 5th Best: Jonathan H. (DBS)
+Overall 15th Best: Pacey Q. (Dulwich)
+Overall 18th Best: Aiden T. (CIS)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -5733,6 +5805,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -5824,10 +5904,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5882,11 +5963,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -6159,11 +6250,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1001"/>
+  <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6230,93 +6321,89 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="176" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:27" ht="395" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="F2" s="21">
+        <v>1</v>
+      </c>
+      <c r="G2" s="21">
+        <v>0</v>
+      </c>
+      <c r="H2" s="21">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="I2" s="21">
+        <v>0</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+    </row>
+    <row r="3" spans="1:27" ht="176" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>3</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-    </row>
-    <row r="3" spans="1:27" ht="208" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
       </c>
       <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
         <v>3</v>
       </c>
-      <c r="H3" s="6">
-        <v>11</v>
-      </c>
       <c r="I3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -6332,40 +6419,44 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="80" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H4" s="6">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -6381,44 +6472,40 @@
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="408" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -6434,43 +6521,43 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="70" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" ht="408" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="6">
         <v>1</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -6487,21 +6574,21 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="272" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" ht="70" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -6510,19 +6597,21 @@
         <v>0</v>
       </c>
       <c r="H7" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -6538,21 +6627,21 @@
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="112.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" ht="272" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -6561,16 +6650,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -6589,39 +6678,39 @@
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" ht="112.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="G9" s="6">
-        <v>2</v>
-      </c>
-      <c r="H9" s="6">
-        <v>3</v>
-      </c>
       <c r="I9" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -6640,36 +6729,40 @@
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="80" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
         <v>2</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <v>3</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>1</v>
       </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -6687,27 +6780,27 @@
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
     </row>
-    <row r="11" spans="1:27" ht="128" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H11" s="6">
         <v>1</v>
@@ -6715,12 +6808,8 @@
       <c r="I11" s="6">
         <v>0</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -6738,39 +6827,39 @@
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
     </row>
-    <row r="12" spans="1:27" ht="80" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" ht="128" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
       </c>
       <c r="H12" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -6789,21 +6878,21 @@
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
     </row>
-    <row r="13" spans="1:27" ht="192" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -6812,16 +6901,16 @@
         <v>1</v>
       </c>
       <c r="H13" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I13" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -6840,21 +6929,21 @@
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
     </row>
-    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -6863,13 +6952,17 @@
         <v>1</v>
       </c>
       <c r="H14" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I14" s="6">
         <v>0</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -6887,18 +6980,34 @@
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
     </row>
-    <row r="15" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="16">
-        <v>2024</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="3"/>
@@ -6918,40 +7027,20 @@
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
     </row>
-    <row r="16" spans="1:27" ht="219.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6">
-        <v>3</v>
-      </c>
-      <c r="H16" s="6">
-        <v>10</v>
-      </c>
-      <c r="I16" s="6">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>105</v>
-      </c>
+    <row r="16" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="16">
+        <v>2024</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -6969,36 +7058,40 @@
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
     </row>
-    <row r="17" spans="1:27" ht="80" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:27" ht="219.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17" s="6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I17" s="6">
         <v>1</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="J17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -7016,21 +7109,21 @@
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
     </row>
-    <row r="18" spans="1:27" ht="208" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>268</v>
+        <v>108</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -7039,18 +7132,14 @@
         <v>2</v>
       </c>
       <c r="H18" s="6">
+        <v>4</v>
+      </c>
+      <c r="I18" s="6">
         <v>1</v>
       </c>
-      <c r="I18" s="6">
-        <v>0</v>
-      </c>
       <c r="J18" s="6"/>
-      <c r="K18" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>267</v>
-      </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -7067,41 +7156,41 @@
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
     </row>
-    <row r="19" spans="1:27" ht="176" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>268</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="6">
         <v>2</v>
       </c>
       <c r="H19" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I19" s="6">
-        <v>1</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L19" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -7118,36 +7207,40 @@
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
     </row>
-    <row r="20" spans="1:27" ht="80" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:27" ht="176" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I20" s="6">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -7165,40 +7258,36 @@
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
     </row>
-    <row r="21" spans="1:27" ht="128" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I21" s="6">
         <v>0</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>133</v>
-      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -7216,21 +7305,21 @@
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
     </row>
-    <row r="22" spans="1:27" ht="192" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:27" ht="128" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -7239,14 +7328,16 @@
         <v>1</v>
       </c>
       <c r="H22" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I22" s="6">
         <v>0</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="J22" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="K22" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -7267,19 +7358,19 @@
     </row>
     <row r="23" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -7288,16 +7379,14 @@
         <v>1</v>
       </c>
       <c r="H23" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I23" s="6">
-        <v>1</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>132</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J23" s="6"/>
       <c r="K23" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -7316,36 +7405,40 @@
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
     </row>
-    <row r="24" spans="1:27" ht="16" x14ac:dyDescent="0.15">
-      <c r="A24" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0</v>
+    <row r="24" spans="1:27" ht="192" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
       </c>
       <c r="G24" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="6">
+        <v>4</v>
+      </c>
+      <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="I24" s="6">
-        <v>0</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="J24" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -7363,30 +7456,30 @@
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
     </row>
-    <row r="25" spans="1:27" ht="64" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="4">
+    <row r="25" spans="1:27" ht="16" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="6">
         <v>0</v>
       </c>
       <c r="G25" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="6">
         <v>0</v>
@@ -7410,38 +7503,36 @@
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
     </row>
-    <row r="26" spans="1:27" ht="96" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:27" ht="64" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="F26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I26" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26" s="6"/>
-      <c r="K26" s="6" t="s">
-        <v>160</v>
-      </c>
+      <c r="K26" s="6"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -7459,37 +7550,37 @@
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
     </row>
-    <row r="27" spans="1:27" ht="160" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:27" ht="96" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="6">
         <v>1</v>
       </c>
       <c r="H27" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I27" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -7508,36 +7599,38 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
     </row>
-    <row r="28" spans="1:27" ht="144" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:27" ht="160" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F28" s="4">
         <v>0</v>
       </c>
       <c r="G28" s="6">
+        <v>1</v>
+      </c>
+      <c r="H28" s="6">
         <v>0</v>
-      </c>
-      <c r="H28" s="6">
-        <v>1</v>
       </c>
       <c r="I28" s="6">
         <v>0</v>
       </c>
       <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -7555,38 +7648,36 @@
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="272" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" s="6">
+    <row r="29" spans="1:27" ht="144" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
         <v>1</v>
       </c>
-      <c r="G29" s="6">
-        <v>1</v>
-      </c>
-      <c r="H29" s="6">
-        <v>9</v>
-      </c>
       <c r="I29" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J29" s="6"/>
-      <c r="K29" s="6" t="s">
-        <v>176</v>
-      </c>
+      <c r="K29" s="6"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -7604,21 +7695,21 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="144" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:27" ht="272" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F30" s="6">
         <v>1</v>
@@ -7627,14 +7718,14 @@
         <v>1</v>
       </c>
       <c r="H30" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I30" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -7653,37 +7744,37 @@
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="80" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:27" ht="144" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F31" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="6">
         <v>1</v>
       </c>
       <c r="H31" s="6">
+        <v>7</v>
+      </c>
+      <c r="I31" s="6">
         <v>2</v>
-      </c>
-      <c r="I31" s="6">
-        <v>0</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -7702,27 +7793,27 @@
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
     </row>
-    <row r="32" spans="1:27" ht="304" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>266</v>
+        <v>187</v>
       </c>
       <c r="F32" s="6">
         <v>0</v>
       </c>
       <c r="G32" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="6">
         <v>2</v>
@@ -7732,7 +7823,7 @@
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -7751,37 +7842,37 @@
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
     </row>
-    <row r="33" spans="1:27" ht="176" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F33" s="4">
+    <row r="33" spans="1:27" ht="304" x14ac:dyDescent="0.15">
+      <c r="A33" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F33" s="6">
         <v>0</v>
       </c>
       <c r="G33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="6">
         <v>0</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -7800,37 +7891,37 @@
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
     </row>
-    <row r="34" spans="1:27" ht="208" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F34" s="6">
-        <v>1</v>
+    <row r="34" spans="1:27" ht="176" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
       </c>
       <c r="G34" s="6">
         <v>1</v>
       </c>
       <c r="H34" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I34" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -7849,21 +7940,21 @@
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
     </row>
-    <row r="35" spans="1:27" ht="176" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F35" s="6">
         <v>1</v>
@@ -7872,14 +7963,14 @@
         <v>1</v>
       </c>
       <c r="H35" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I35" s="6">
         <v>1</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -7898,21 +7989,21 @@
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
     </row>
-    <row r="36" spans="1:27" ht="192" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:27" ht="176" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F36" s="6">
         <v>1</v>
@@ -7921,14 +8012,14 @@
         <v>1</v>
       </c>
       <c r="H36" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I36" s="6">
         <v>1</v>
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -7947,37 +8038,37 @@
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
     </row>
-    <row r="37" spans="1:27" ht="240" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F37" s="6">
         <v>1</v>
       </c>
       <c r="G37" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I37" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -7996,37 +8087,37 @@
       <c r="Z37" s="3"/>
       <c r="AA37" s="3"/>
     </row>
-    <row r="38" spans="1:27" ht="208" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:27" ht="240" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F38" s="6">
         <v>1</v>
       </c>
       <c r="G38" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H38" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I38" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -8045,37 +8136,37 @@
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
     </row>
-    <row r="39" spans="1:27" ht="192" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="6">
+        <v>3</v>
+      </c>
+      <c r="H39" s="6">
         <v>1</v>
       </c>
-      <c r="H39" s="6">
-        <v>7</v>
-      </c>
       <c r="I39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -8094,37 +8185,37 @@
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
     </row>
-    <row r="40" spans="1:27" ht="176" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>89</v>
+        <v>232</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F40" s="6">
         <v>0</v>
       </c>
       <c r="G40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I40" s="6">
         <v>0</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -8143,30 +8234,38 @@
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
     </row>
-    <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="2">
-        <f t="shared" ref="F41:I41" si="0">SUM(F16:F40)</f>
-        <v>13</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="H41" s="2">
-        <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="I41" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
+    <row r="41" spans="1:27" ht="176" x14ac:dyDescent="0.15">
+      <c r="A41" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" s="6">
+        <v>0</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0</v>
+      </c>
+      <c r="H41" s="6">
+        <v>2</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0</v>
       </c>
       <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6" t="s">
+        <v>240</v>
+      </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -8185,17 +8284,29 @@
       <c r="AA41" s="3"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="2">
+        <f t="shared" ref="F42:I42" si="0">SUM(F17:F41)</f>
+        <v>13</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -13984,7 +14095,35 @@
       <c r="Z241" s="3"/>
       <c r="AA241" s="3"/>
     </row>
-    <row r="242" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
+      <c r="C242" s="3"/>
+      <c r="D242" s="3"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
+      <c r="H242" s="3"/>
+      <c r="I242" s="3"/>
+      <c r="J242" s="3"/>
+      <c r="K242" s="3"/>
+      <c r="L242" s="3"/>
+      <c r="M242" s="3"/>
+      <c r="N242" s="3"/>
+      <c r="O242" s="3"/>
+      <c r="P242" s="3"/>
+      <c r="Q242" s="3"/>
+      <c r="R242" s="3"/>
+      <c r="S242" s="3"/>
+      <c r="T242" s="3"/>
+      <c r="U242" s="3"/>
+      <c r="V242" s="3"/>
+      <c r="W242" s="3"/>
+      <c r="X242" s="3"/>
+      <c r="Y242" s="3"/>
+      <c r="Z242" s="3"/>
+      <c r="AA242" s="3"/>
+    </row>
     <row r="243" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="244" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="245" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14744,52 +14883,54 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:I16"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C36" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C37" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C38" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C39" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C40" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C41" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C2" r:id="rId38" xr:uid="{5B52365D-90D7-BA42-A558-C08D923BA6CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Set up baseline snapshot for weekly leaderboard tracking
- Create baseline snapshot from current spreadsheet state (June 15, 2025)
- Modify position change logic to show no changes for baseline week
- Add create-baseline-snapshot.js script for future baseline resets
- Install node-fetch dependency for snapshot scripts
- Update CLAUDE.md with snapshot management documentation

System now ready for weekly position tracking:
- Baseline: All students show dash (—) for no change
- Future weeks: Will show green/red arrows for position changes
- Automatic weekly snapshots every Sunday

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/debate_achievements.xlsx
+++ b/data/debate_achievements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tikaram/Downloads/Claude Code/students/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F0187B-2D2C-C842-95F6-7BE705E9071C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A6C07E-D82B-B847-ACE6-3B52268D2862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,12 +401,6 @@
     </r>
   </si>
   <si>
-    <t>Huge congratulations to our debaters for their outstanding performance at the South Asian Schools Debating Championship 2025, held from June 6-8!
-Congratulations to Emi R. (CIS) and Tony S. (CIS) for reaching the Quarterfinals! Well done also to Aiden T. (CIS), Bella L. (CIS), and Pacey Q. (Dulwich) for making it to the Octofinals.
-Further accolades go to our students who earned individual speaker awards. Congratulations to Emi R. (CIS) for being the Overall 5th Best Speaker, Tony S. (CIS) for being the Overall 12th Best Speaker, and Pacey Q. (Dulwich) for being the Overall 13th Best Speaker.
-We are incredibly proud of all our debaters for their hard work, dedication, and commitment. We look forward to seeing your continued growth and success.</t>
-  </si>
-  <si>
     <t>South Asia Schools BP</t>
   </si>
   <si>
@@ -5655,53 +5649,16 @@
     <t>https://asdc2025.calicotab.com/asdc2025/</t>
   </si>
   <si>
-    <t>We are thrilled to announce the outstanding results of our debaters at the Asian Schools Debating Championship ASDC (2025), held from June 16-18!
-A huge congratulations to our Novice Champions: Adrian W. (HKIS), Audrey L. (HKIS), and Ryan Q. (HKIS)! This is a fantastic achievement and a testament to their hard work and skill.
-Further congratulations to the students who reached the Quarterfinals: Aiden T. (CIS), Jonathan H. (DBS), Pacey Q. (Dulwich), Samuel K. (CIS), Vir K. (HKIS), CECILIA L. (BISOG), and Theodore W. (HKIS). Reaching the elimination rounds in such a competitive tournament is a significant accomplishment.
-Our debaters also earned numerous individual speaker awards across various categories.
-In the Junior category, congratulations to Theodore W. (HKIS) for placing 3rd, CECILIA L. (BISOG) for 4th, Aiden T. (CIS) for 7th, and Samuel K. (CIS) for 8th Best Speaker.
-In the Novice category, well done to Jonathan H. (DBS) for 2nd, Theodore W. (HKIS) for 5th, CECILIA L. (BISOG) for 6th, Pacey Q. (Dulwich) for 8th, Aiden T. (CIS) for 11th, Samuel K. (CIS) for 13th, and Vir K. (HKIS) for 15th Best Speaker.
-In the Overall rankings, congratulations to Jonathan H. (DBS) for placing 5th, Theodore W. (HKIS) for 12th, CECILIA L. (BISOG) for 13th, Pacey Q. (Dulwich) for 15th, and Aiden T. (CIS) for 18th Best Speaker.
-We are incredibly proud of all our debaters for their dedication, perseverance, and exceptional performance at ASDC 2025. These results reflect their commitment to excellence. Well done everyone!</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Novice Champions:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="EB Garamond"/>
-      </rPr>
-      <t>Adrian W. (HKIS)
+    <t>Novice Champions:
+Adrian W. (HKIS)
 Audrey L. (HKIS)
-Ryan Q. (HKIS)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="EB Garamond"/>
-      </rPr>
-      <t xml:space="preserve">
+Ryan Q. (HKIS)
 Quarterfinalists:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="EB Garamond"/>
-      </rPr>
-      <t>Aiden T. (CIS)
+Aiden T. (CIS)
 Jonathan H. (DBS)
-Pacey Q. (Dulwich)
+Pacey Q. (DCB)
 Samuel K. (CIS)
 Vir K. (HKIS)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">
@@ -5709,13 +5666,29 @@
 Junior 8th Best: Samuel K. (CIS)
 Novice 2nd Best: Jonathan H. (DBS)
 Novice 5th Best: Theodore W. (HKIS)
-Novice 8th Best: Pacey Q. (Dulwich)
+Novice 8th Best: Pacey Q. (DCB)
 Novice 11th Best: Aiden T. (CIS)
 Novice 13th Best: Samuel K. (CIS)
 Novice 15th Best: Vir K. (HKIS)
 Overall 5th Best: Jonathan H. (DBS)
-Overall 15th Best: Pacey Q. (Dulwich)
+Overall 15th Best: Pacey Q. (DCB)
 Overall 18th Best: Aiden T. (CIS)</t>
+  </si>
+  <si>
+    <t>We are thrilled to announce the outstanding results of our debaters at the Asian Schools Debating Championship ASDC (2025), held from June 16-18!
+A huge congratulations to our Novice Champions: Adrian W. (HKIS), Audrey L. (HKIS), and Ryan Q. (HKIS)! This is a fantastic achievement and a testament to their hard work and skill.
+Further congratulations to the students who reached the Quarterfinals: Aiden T. (CIS), Jonathan H. (DBS), Pacey Q. (DCB), Samuel K. (CIS), Vir K. (HKIS), CECILIA L. (BISOG), and Theodore W. (HKIS). Reaching the elimination rounds in such a competitive tournament is a significant accomplishment.
+Our debaters also earned numerous individual speaker awards across various categories.
+In the Junior category, congratulations to Theodore W. (HKIS) for placing 3rd, CECILIA L. (BISOG) for 4th, Aiden T. (CIS) for 7th, and Samuel K. (CIS) for 8th Best Speaker.
+In the Novice category, well done to Jonathan H. (DBS) for 2nd, Theodore W. (HKIS) for 5th, CECILIA L. (BISOG) for 6th, Pacey Q. (DCB) for 8th, Aiden T. (CIS) for 11th, Samuel K. (CIS) for 13th, and Vir K. (HKIS) for 15th Best Speaker.
+In the Overall rankings, congratulations to Jonathan H. (DBS) for placing 5th, Theodore W. (HKIS) for 12th, CECILIA L. (BISOG) for 13th, Pacey Q. (DCB) for 15th, and Aiden T. (CIS) for 18th Best Speaker.
+We are incredibly proud of all our debaters for their dedication, perseverance, and exceptional performance at ASDC 2025. These results reflect their commitment to excellence. Well done everyone!</t>
+  </si>
+  <si>
+    <t>Huge congratulations to our debaters for their outstanding performance at the South Asian Schools Debating Championship 2025, held from June 6-8!
+Congratulations to Emi R. (CIS) and Tony S. (CIS) for reaching the Quarterfinals! Well done also to Aiden T. (CIS), Bella L. (CIS), and Pacey Q. (DCB) for making it to the Octofinals.
+Further accolades go to our students who earned individual speaker awards. Congratulations to Emi R. (CIS) for being the Overall 5th Best Speaker, Tony S. (CIS) for being the Overall 12th Best Speaker, and Pacey Q. (DCB) for being the Overall 13th Best Speaker.
+We are incredibly proud of all our debaters for their hard work, dedication, and commitment. We look forward to seeing your continued growth and success.</t>
   </si>
 </sst>
 </file>
@@ -6254,7 +6227,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6321,21 +6294,21 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="395" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="380" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>273</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F2" s="21">
         <v>1</v>
@@ -6351,7 +6324,7 @@
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
@@ -6400,7 +6373,7 @@
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>16</v>
+        <v>274</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -6421,19 +6394,19 @@
     </row>
     <row r="4" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -6449,13 +6422,13 @@
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -6474,19 +6447,19 @@
     </row>
     <row r="5" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
@@ -6502,7 +6475,7 @@
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -6523,19 +6496,19 @@
     </row>
     <row r="6" spans="1:27" ht="408" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -6551,13 +6524,13 @@
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -6576,19 +6549,19 @@
     </row>
     <row r="7" spans="1:27" ht="70" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -6604,13 +6577,13 @@
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -6629,19 +6602,19 @@
     </row>
     <row r="8" spans="1:27" ht="272" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -6656,10 +6629,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -6680,19 +6653,19 @@
     </row>
     <row r="9" spans="1:27" ht="112.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -6707,10 +6680,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -6731,19 +6704,19 @@
     </row>
     <row r="10" spans="1:27" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -6758,10 +6731,10 @@
         <v>1</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -6782,19 +6755,19 @@
     </row>
     <row r="11" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -6829,19 +6802,19 @@
     </row>
     <row r="12" spans="1:27" ht="128" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -6856,10 +6829,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -6880,19 +6853,19 @@
     </row>
     <row r="13" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -6907,10 +6880,10 @@
         <v>2</v>
       </c>
       <c r="J13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -6931,19 +6904,19 @@
     </row>
     <row r="14" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -6958,10 +6931,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -6982,19 +6955,19 @@
     </row>
     <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
@@ -7060,19 +7033,19 @@
     </row>
     <row r="17" spans="1:27" ht="219.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
@@ -7087,10 +7060,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -7111,19 +7084,19 @@
     </row>
     <row r="18" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="F18" s="4">
         <v>0</v>
@@ -7158,19 +7131,19 @@
     </row>
     <row r="19" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="D19" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -7186,10 +7159,10 @@
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -7209,19 +7182,19 @@
     </row>
     <row r="20" spans="1:27" ht="176" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -7236,10 +7209,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K20" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -7260,19 +7233,19 @@
     </row>
     <row r="21" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -7307,19 +7280,19 @@
     </row>
     <row r="22" spans="1:27" ht="128" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -7334,10 +7307,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -7358,19 +7331,19 @@
     </row>
     <row r="23" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -7386,7 +7359,7 @@
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -7407,19 +7380,19 @@
     </row>
     <row r="24" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -7434,10 +7407,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -7458,19 +7431,19 @@
     </row>
     <row r="25" spans="1:27" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="E25" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
@@ -7505,19 +7478,19 @@
     </row>
     <row r="26" spans="1:27" ht="64" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="E26" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F26" s="4">
         <v>0</v>
@@ -7552,19 +7525,19 @@
     </row>
     <row r="27" spans="1:27" ht="96" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
@@ -7580,7 +7553,7 @@
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -7601,19 +7574,19 @@
     </row>
     <row r="28" spans="1:27" ht="160" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>164</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" s="4">
         <v>0</v>
@@ -7629,7 +7602,7 @@
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -7650,19 +7623,19 @@
     </row>
     <row r="29" spans="1:27" ht="144" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>170</v>
       </c>
       <c r="F29" s="4">
         <v>0</v>
@@ -7697,19 +7670,19 @@
     </row>
     <row r="30" spans="1:27" ht="272" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="F30" s="6">
         <v>1</v>
@@ -7725,7 +7698,7 @@
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -7746,19 +7719,19 @@
     </row>
     <row r="31" spans="1:27" ht="144" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="F31" s="6">
         <v>1</v>
@@ -7774,7 +7747,7 @@
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -7795,19 +7768,19 @@
     </row>
     <row r="32" spans="1:27" ht="80" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="F32" s="6">
         <v>0</v>
@@ -7823,7 +7796,7 @@
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -7844,19 +7817,19 @@
     </row>
     <row r="33" spans="1:27" ht="304" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="C33" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="E33" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F33" s="6">
         <v>0</v>
@@ -7872,7 +7845,7 @@
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -7893,19 +7866,19 @@
     </row>
     <row r="34" spans="1:27" ht="176" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="F34" s="4">
         <v>0</v>
@@ -7921,7 +7894,7 @@
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -7942,19 +7915,19 @@
     </row>
     <row r="35" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="F35" s="6">
         <v>1</v>
@@ -7970,7 +7943,7 @@
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -7991,19 +7964,19 @@
     </row>
     <row r="36" spans="1:27" ht="176" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="F36" s="6">
         <v>1</v>
@@ -8019,7 +7992,7 @@
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -8040,19 +8013,19 @@
     </row>
     <row r="37" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="F37" s="6">
         <v>1</v>
@@ -8068,7 +8041,7 @@
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -8089,19 +8062,19 @@
     </row>
     <row r="38" spans="1:27" ht="240" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="C38" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="F38" s="6">
         <v>1</v>
@@ -8117,7 +8090,7 @@
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -8138,19 +8111,19 @@
     </row>
     <row r="39" spans="1:27" ht="208" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="D39" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="F39" s="6">
         <v>1</v>
@@ -8166,7 +8139,7 @@
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -8187,19 +8160,19 @@
     </row>
     <row r="40" spans="1:27" ht="192" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="D40" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="F40" s="6">
         <v>0</v>
@@ -8215,7 +8188,7 @@
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -8236,19 +8209,19 @@
     </row>
     <row r="41" spans="1:27" ht="176" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="C41" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="F41" s="6">
         <v>0</v>
@@ -8264,7 +8237,7 @@
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -14952,10 +14925,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>241</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>242</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -14984,10 +14957,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>244</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -15016,10 +14989,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>245</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>246</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -15048,10 +15021,10 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>247</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>248</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15080,10 +15053,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>250</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -15112,10 +15085,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>252</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -15144,13 +15117,13 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>255</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -15178,10 +15151,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>257</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -15210,10 +15183,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>258</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>259</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -15242,10 +15215,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -15274,10 +15247,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -21962,7 +21935,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -21971,7 +21944,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Improve ASDC tournament recognition for 2× multiplier
- Update isMajorTournament() to recognize full tournament names
- Add support for "Asian Schools Debating Championship" variations
- Include "South Asian Schools Debating Championship" recognition
- Maintain support for abbreviated forms (ASDC, WSDC)

Results:
- ASDC 2025 achievements now properly receive 2× points multiplier
- Novice Champion: 30 → 60 points
- Quarterfinalist: 15 → 30 points
- All ASDC speaker awards doubled appropriately

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/debate_achievements.xlsx
+++ b/data/debate_achievements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tikaram/Downloads/Claude Code/students/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A6C07E-D82B-B847-ACE6-3B52268D2862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15B2FED-5F59-5F44-9559-5F24BD46E05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6227,7 +6227,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Fix major tournament recognition to be exact matches only
- Remove overly broad matching that incorrectly identified regional tournaments
- Only ASDC variants get 2× multiplier: "Asian Schools Debating Championship", "South Asian Schools Debating Championship"
- Regional tournaments like "South Asia WSDC", "Everest WSDC", "Doxbridge WSDC" correctly get 1× multiplier
- Maintain exact pattern matching for future WSDC tournaments

Fixes incorrect 2× multiplier assignment to:
- Everest International World Schools Debating Championship
- South Asia WSDC (regional qualifier, not actual WSDC)
- Other regional WSDC tournaments

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/debate_achievements.xlsx
+++ b/data/debate_achievements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tikaram/Downloads/Claude Code/students/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15B2FED-5F59-5F44-9559-5F24BD46E05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5914D77-4BBB-864B-89D9-6654B640EBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6227,7 +6227,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>